<commit_message>
Upload Jobsheet 10_Praktikum 1
</commit_message>
<xml_diff>
--- a/public/template_detail.xlsx
+++ b/public/template_detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56FF1B5F-6DC8-40F1-A2B1-07FDC0A85892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8889F74-E920-49EE-A1F7-B1476A3C0C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="12" windowWidth="23004" windowHeight="12948" xr2:uid="{944EC1E6-4F90-4417-9D19-0F0BB9EE3CBC}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DCEA1C-48FD-4793-A23F-BF6879E3849F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,58 +416,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>500000</v>
+        <v>10000</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1100000</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>300000</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>300000</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>